<commit_message>
add merge data code
</commit_message>
<xml_diff>
--- a/SecondaryData.xlsx
+++ b/SecondaryData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wichu\Documents\GitHub\DataAnalysis_AJarnJA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc8a30ddd1064f63/Documents/GitHub/HeatStandard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48635697-871D-4454-A573-552671D43E85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{48635697-871D-4454-A573-552671D43E85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D2BFBD23-73DE-4A8E-A6A0-3772E24E9E70}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ข้อมูล secondary" sheetId="1" r:id="rId1"/>
@@ -1920,10 +1920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ300"/>
+  <dimension ref="A1:AMJ297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P128" sqref="O128:P128"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="24" x14ac:dyDescent="0.8"/>
@@ -19824,12 +19824,6 @@
         <v>33</v>
       </c>
     </row>
-    <row r="300" spans="1:24" x14ac:dyDescent="0.8">
-      <c r="B300" s="2">
-        <f>SUBTOTAL(3,N:N)</f>
-        <v>256</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>